<commit_message>
Updates to template and fix of standard run mode
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.Payments.MetricsGeneration/Resources/MetricsTemplate.xlsx
+++ b/src/SFA.DAS.Payments.MetricsGeneration/Resources/MetricsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkKeene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\das-payments-V2-validation\src\SFA.DAS.Payments.MetricsGeneration\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C6F585D-6779-409B-9EF2-1A1611B0F549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D39A9C-864F-4D97-85AF-AE4FB14CF01E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6804" yWindow="-17388" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAS Payments" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Required Payments made this month</t>
   </si>
@@ -87,17 +87,21 @@
   </si>
   <si>
     <t>HBCP</t>
+  </si>
+  <si>
+    <t>Payments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +125,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,21 +176,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -485,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -642,10 +665,38 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7">
+        <f>G5+H5+C9</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="9" t="e">
+        <f>C18/B2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="9" t="e">
+        <f>C18/A2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -788,18 +839,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,6 +872,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F95D9D9-2345-4A14-B5CA-9F1E06E63601}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8FF543-4B0C-4924-BCE4-8A51F7F1551C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -834,12 +893,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F95D9D9-2345-4A14-B5CA-9F1E06E63601}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>